<commit_message>
Added continue and pause of drive
</commit_message>
<xml_diff>
--- a/05_design/communication_protocol_MCU_NavU/com_protocol_MCU_NavU.xlsx
+++ b/05_design/communication_protocol_MCU_NavU/com_protocol_MCU_NavU.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Volumes/Macintosh SD/Github/ADAS/05_design/communication_protocol_MCU_NavU/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AB5A88E6-612B-214D-8927-615F0B881EF9}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EB8E4C05-2459-3B46-A745-BC03D350CA38}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5340" yWindow="1100" windowWidth="22600" windowHeight="17440" xr2:uid="{17E85F93-DC07-064E-BD90-F4BCCAC86647}"/>
+    <workbookView xWindow="6520" yWindow="460" windowWidth="22600" windowHeight="17440" activeTab="1" xr2:uid="{17E85F93-DC07-064E-BD90-F4BCCAC86647}"/>
   </bookViews>
   <sheets>
     <sheet name="Structure" sheetId="1" r:id="rId1"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="57">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="63">
   <si>
     <t>To exchange data between the Navigation Unit (NavU) and the Motor Control Unit (MCU) a serial communication protocol is used.</t>
   </si>
@@ -204,6 +204,24 @@
   </si>
   <si>
     <t>Inter-Controller Communication Protocol NavU &lt;&gt; MCU</t>
+  </si>
+  <si>
+    <t>Pause Drive</t>
+  </si>
+  <si>
+    <t>0x06</t>
+  </si>
+  <si>
+    <t>Command to pause movement.</t>
+  </si>
+  <si>
+    <t>Continue Drive</t>
+  </si>
+  <si>
+    <t>0x07</t>
+  </si>
+  <si>
+    <t>Command to continue movement.</t>
   </si>
 </sst>
 </file>
@@ -269,7 +287,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="4">
     <border>
       <left/>
       <right/>
@@ -292,11 +310,37 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="22">
+  <cellXfs count="26">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -353,11 +397,29 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="12">
+    <dxf>
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
     <dxf>
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
@@ -391,12 +453,6 @@
         <scheme val="minor"/>
       </font>
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
@@ -440,32 +496,32 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{89E501DF-FC80-5A42-9DB0-2D7A474EAA23}" name="Table1" displayName="Table1" ref="A3:E9" totalsRowShown="0" headerRowDxfId="11">
-  <autoFilter ref="A3:E9" xr:uid="{04D97AA9-83CD-F341-B287-B8A125F374D0}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{89E501DF-FC80-5A42-9DB0-2D7A474EAA23}" name="Table1" displayName="Table1" ref="A3:E11" totalsRowShown="0" headerRowDxfId="11">
+  <autoFilter ref="A3:E11" xr:uid="{04D97AA9-83CD-F341-B287-B8A125F374D0}"/>
   <tableColumns count="5">
     <tableColumn id="1" xr3:uid="{FF9667FF-DB1E-D44E-A164-C4FB77F35094}" name="Name:" dataDxfId="10"/>
     <tableColumn id="2" xr3:uid="{A30118A6-7AAE-4643-AC4E-BB820D349C15}" name="CMD:" dataDxfId="9"/>
     <tableColumn id="3" xr3:uid="{41E328FC-0957-4140-99A9-8968EBEC9AA1}" name="Data:" dataDxfId="8"/>
-    <tableColumn id="4" xr3:uid="{8CC32685-8E72-A540-9D03-09723D9F1966}" name="Data range:" dataDxfId="7">
+    <tableColumn id="4" xr3:uid="{8CC32685-8E72-A540-9D03-09723D9F1966}" name="Data range:" dataDxfId="1">
       <calculatedColumnFormula>"-1 and 1"</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="5" xr3:uid="{4B37721B-7B89-D947-9B44-FE7C23298BE3}" name="Description:" dataDxfId="6"/>
+    <tableColumn id="5" xr3:uid="{4B37721B-7B89-D947-9B44-FE7C23298BE3}" name="Description:" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium6" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{58402A27-822A-D844-A4E0-2AEE8F6F98D3}" name="Table13" displayName="Table13" ref="A3:E6" totalsRowShown="0" headerRowDxfId="5">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{58402A27-822A-D844-A4E0-2AEE8F6F98D3}" name="Table13" displayName="Table13" ref="A3:E6" totalsRowShown="0" headerRowDxfId="7">
   <autoFilter ref="A3:E6" xr:uid="{6A40FC90-759C-6140-8009-1917E148D860}"/>
   <tableColumns count="5">
-    <tableColumn id="1" xr3:uid="{74A0A924-7A74-1B41-92AF-789ACB410B08}" name="Name:" dataDxfId="4"/>
-    <tableColumn id="2" xr3:uid="{1E5232E9-CE19-134F-AE49-E89F5B483440}" name="CMD:" dataDxfId="3"/>
-    <tableColumn id="3" xr3:uid="{A600437B-AA69-2648-A607-CB0E1E58B896}" name="Data:" dataDxfId="2"/>
-    <tableColumn id="4" xr3:uid="{323638DE-F781-3844-A115-EE83E4F878D5}" name="Data range:" dataDxfId="1">
+    <tableColumn id="1" xr3:uid="{74A0A924-7A74-1B41-92AF-789ACB410B08}" name="Name:" dataDxfId="6"/>
+    <tableColumn id="2" xr3:uid="{1E5232E9-CE19-134F-AE49-E89F5B483440}" name="CMD:" dataDxfId="5"/>
+    <tableColumn id="3" xr3:uid="{A600437B-AA69-2648-A607-CB0E1E58B896}" name="Data:" dataDxfId="4"/>
+    <tableColumn id="4" xr3:uid="{323638DE-F781-3844-A115-EE83E4F878D5}" name="Data range:" dataDxfId="3">
       <calculatedColumnFormula>"-1 and 1"</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="5" xr3:uid="{7DF12235-1193-B146-9500-65AAD177040D}" name="Description:" dataDxfId="0"/>
+    <tableColumn id="5" xr3:uid="{7DF12235-1193-B146-9500-65AAD177040D}" name="Description:" dataDxfId="2"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium6" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -770,8 +826,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CEAB2FAD-92B8-DB4D-AB4C-9159AFD8911A}">
   <dimension ref="A1:G16"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B29" sqref="B29"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D29" sqref="D29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -792,7 +848,7 @@
       </c>
       <c r="G1" s="19">
         <f ca="1">NOW()</f>
-        <v>43482.369223379632</v>
+        <v>43483.434360069441</v>
       </c>
     </row>
     <row r="3" spans="1:7" ht="36" customHeight="1" x14ac:dyDescent="0.2">
@@ -818,36 +874,40 @@
       <c r="B8" s="13">
         <v>0</v>
       </c>
-      <c r="C8" s="17">
+      <c r="C8" s="13">
         <v>1</v>
       </c>
-      <c r="D8" s="15">
+      <c r="D8" s="17">
         <v>2</v>
       </c>
       <c r="E8" s="15">
         <v>3</v>
       </c>
-      <c r="F8" s="13">
+      <c r="F8" s="15">
         <v>4</v>
+      </c>
+      <c r="G8" s="13">
+        <v>5</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A9" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="B9" s="13" t="s">
+      <c r="B9" s="22" t="s">
         <v>18</v>
       </c>
-      <c r="C9" s="17" t="s">
+      <c r="C9" s="23"/>
+      <c r="D9" s="17" t="s">
         <v>6</v>
       </c>
-      <c r="D9" s="15" t="s">
+      <c r="E9" s="15" t="s">
         <v>7</v>
       </c>
-      <c r="E9" s="15" t="s">
+      <c r="F9" s="15" t="s">
         <v>8</v>
       </c>
-      <c r="F9" s="13" t="s">
+      <c r="G9" s="13" t="s">
         <v>19</v>
       </c>
     </row>
@@ -858,16 +918,19 @@
       <c r="B10" s="13" t="s">
         <v>9</v>
       </c>
-      <c r="C10" s="17" t="s">
-        <v>10</v>
-      </c>
-      <c r="D10" s="15" t="s">
+      <c r="C10" s="13" t="s">
+        <v>9</v>
+      </c>
+      <c r="D10" s="17" t="s">
         <v>10</v>
       </c>
       <c r="E10" s="15" t="s">
         <v>10</v>
       </c>
-      <c r="F10" s="13" t="s">
+      <c r="F10" s="15" t="s">
+        <v>10</v>
+      </c>
+      <c r="G10" s="13" t="s">
         <v>11</v>
       </c>
     </row>
@@ -875,19 +938,20 @@
       <c r="A11" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="B11" s="14" t="s">
+      <c r="B11" s="24" t="s">
         <v>12</v>
       </c>
-      <c r="C11" s="18" t="s">
+      <c r="C11" s="25"/>
+      <c r="D11" s="18" t="s">
         <v>13</v>
       </c>
-      <c r="D11" s="16" t="s">
+      <c r="E11" s="16" t="s">
         <v>14</v>
       </c>
-      <c r="E11" s="16" t="s">
+      <c r="F11" s="16" t="s">
         <v>15</v>
       </c>
-      <c r="F11" s="14" t="s">
+      <c r="G11" s="14" t="s">
         <v>16</v>
       </c>
     </row>
@@ -910,9 +974,11 @@
       </c>
     </row>
   </sheetData>
-  <mergeCells count="2">
+  <mergeCells count="4">
     <mergeCell ref="A3:G3"/>
     <mergeCell ref="A1:E1"/>
+    <mergeCell ref="B9:C9"/>
+    <mergeCell ref="B11:C11"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
@@ -921,10 +987,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EFFE341A-F7C8-3F43-AC32-216069D199D4}">
-  <dimension ref="A1:E9"/>
+  <dimension ref="A1:E11"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C13" sqref="C13"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A12" sqref="A12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -971,7 +1037,7 @@
         <f>"-1 and 1"</f>
         <v>-1 and 1</v>
       </c>
-      <c r="E4" s="9" t="s">
+      <c r="E4" s="11" t="s">
         <v>28</v>
       </c>
     </row>
@@ -989,7 +1055,7 @@
         <f>"-32,768 .. 32,767"</f>
         <v>-32,768 .. 32,767</v>
       </c>
-      <c r="E5" s="9" t="s">
+      <c r="E5" s="11" t="s">
         <v>32</v>
       </c>
     </row>
@@ -1007,11 +1073,11 @@
         <f>"-32,768 .. 32,767"</f>
         <v>-32,768 .. 32,767</v>
       </c>
-      <c r="E6" s="9" t="s">
+      <c r="E6" s="11" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="7" spans="1:5" ht="50" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:5" ht="68" x14ac:dyDescent="0.2">
       <c r="A7" s="11" t="s">
         <v>37</v>
       </c>
@@ -1025,7 +1091,7 @@
         <f>"-32,768 .. 32,767"</f>
         <v>-32,768 .. 32,767</v>
       </c>
-      <c r="E7" s="9" t="s">
+      <c r="E7" s="11" t="s">
         <v>43</v>
       </c>
     </row>
@@ -1043,7 +1109,7 @@
         <f>"-32,768 .. 32,767"</f>
         <v>-32,768 .. 32,767</v>
       </c>
-      <c r="E8" s="9" t="s">
+      <c r="E8" s="11" t="s">
         <v>42</v>
       </c>
     </row>
@@ -1061,8 +1127,44 @@
         <f>"-32,768 .. 32,767"</f>
         <v>-32,768 .. 32,767</v>
       </c>
-      <c r="E9" s="9" t="s">
+      <c r="E9" s="11" t="s">
         <v>47</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" ht="50" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A10" s="11" t="s">
+        <v>57</v>
+      </c>
+      <c r="B10" s="12" t="s">
+        <v>58</v>
+      </c>
+      <c r="C10" s="10" t="s">
+        <v>31</v>
+      </c>
+      <c r="D10" s="12" t="str">
+        <f>"-32,768 .. 32,767"</f>
+        <v>-32,768 .. 32,767</v>
+      </c>
+      <c r="E10" s="11" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" ht="50" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A11" s="11" t="s">
+        <v>60</v>
+      </c>
+      <c r="B11" s="12" t="s">
+        <v>61</v>
+      </c>
+      <c r="C11" s="10" t="s">
+        <v>31</v>
+      </c>
+      <c r="D11" s="12" t="str">
+        <f>"-32,768 .. 32,767"</f>
+        <v>-32,768 .. 32,767</v>
+      </c>
+      <c r="E11" s="11" t="s">
+        <v>62</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added inter-controller communication protocol and battery voltage monitor.
</commit_message>
<xml_diff>
--- a/05_design/communication_protocol_MCU_NavU/com_protocol_MCU_NavU.xlsx
+++ b/05_design/communication_protocol_MCU_NavU/com_protocol_MCU_NavU.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11208"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10115"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Volumes/Macintosh SD/Github/ADAS/05_design/communication_protocol_MCU_NavU/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EB8E4C05-2459-3B46-A745-BC03D350CA38}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E49AE96C-7E30-0E48-AF84-FFFBFBB090A9}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="6520" yWindow="460" windowWidth="22600" windowHeight="17440" activeTab="1" xr2:uid="{17E85F93-DC07-064E-BD90-F4BCCAC86647}"/>
+    <workbookView xWindow="9700" yWindow="460" windowWidth="22600" windowHeight="17440" xr2:uid="{17E85F93-DC07-064E-BD90-F4BCCAC86647}"/>
   </bookViews>
   <sheets>
     <sheet name="Structure" sheetId="1" r:id="rId1"/>
@@ -100,9 +100,6 @@
     <t>TTX = Termination of Transmission</t>
   </si>
   <si>
-    <t>The length of message is always 5 bytes including STX and TTX.</t>
-  </si>
-  <si>
     <t>Messages from NavU to MCU</t>
   </si>
   <si>
@@ -222,6 +219,9 @@
   </si>
   <si>
     <t>Command to continue movement.</t>
+  </si>
+  <si>
+    <t>The length of message is always 6 bytes including STX and TTX.</t>
   </si>
 </sst>
 </file>
@@ -415,12 +415,6 @@
   </cellStyles>
   <dxfs count="12">
     <dxf>
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
@@ -453,6 +447,12 @@
         <scheme val="minor"/>
       </font>
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
@@ -502,26 +502,26 @@
     <tableColumn id="1" xr3:uid="{FF9667FF-DB1E-D44E-A164-C4FB77F35094}" name="Name:" dataDxfId="10"/>
     <tableColumn id="2" xr3:uid="{A30118A6-7AAE-4643-AC4E-BB820D349C15}" name="CMD:" dataDxfId="9"/>
     <tableColumn id="3" xr3:uid="{41E328FC-0957-4140-99A9-8968EBEC9AA1}" name="Data:" dataDxfId="8"/>
-    <tableColumn id="4" xr3:uid="{8CC32685-8E72-A540-9D03-09723D9F1966}" name="Data range:" dataDxfId="1">
+    <tableColumn id="4" xr3:uid="{8CC32685-8E72-A540-9D03-09723D9F1966}" name="Data range:" dataDxfId="7">
       <calculatedColumnFormula>"-1 and 1"</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="5" xr3:uid="{4B37721B-7B89-D947-9B44-FE7C23298BE3}" name="Description:" dataDxfId="0"/>
+    <tableColumn id="5" xr3:uid="{4B37721B-7B89-D947-9B44-FE7C23298BE3}" name="Description:" dataDxfId="6"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium6" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{58402A27-822A-D844-A4E0-2AEE8F6F98D3}" name="Table13" displayName="Table13" ref="A3:E6" totalsRowShown="0" headerRowDxfId="7">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{58402A27-822A-D844-A4E0-2AEE8F6F98D3}" name="Table13" displayName="Table13" ref="A3:E6" totalsRowShown="0" headerRowDxfId="5">
   <autoFilter ref="A3:E6" xr:uid="{6A40FC90-759C-6140-8009-1917E148D860}"/>
   <tableColumns count="5">
-    <tableColumn id="1" xr3:uid="{74A0A924-7A74-1B41-92AF-789ACB410B08}" name="Name:" dataDxfId="6"/>
-    <tableColumn id="2" xr3:uid="{1E5232E9-CE19-134F-AE49-E89F5B483440}" name="CMD:" dataDxfId="5"/>
-    <tableColumn id="3" xr3:uid="{A600437B-AA69-2648-A607-CB0E1E58B896}" name="Data:" dataDxfId="4"/>
-    <tableColumn id="4" xr3:uid="{323638DE-F781-3844-A115-EE83E4F878D5}" name="Data range:" dataDxfId="3">
+    <tableColumn id="1" xr3:uid="{74A0A924-7A74-1B41-92AF-789ACB410B08}" name="Name:" dataDxfId="4"/>
+    <tableColumn id="2" xr3:uid="{1E5232E9-CE19-134F-AE49-E89F5B483440}" name="CMD:" dataDxfId="3"/>
+    <tableColumn id="3" xr3:uid="{A600437B-AA69-2648-A607-CB0E1E58B896}" name="Data:" dataDxfId="2"/>
+    <tableColumn id="4" xr3:uid="{323638DE-F781-3844-A115-EE83E4F878D5}" name="Data range:" dataDxfId="1">
       <calculatedColumnFormula>"-1 and 1"</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="5" xr3:uid="{7DF12235-1193-B146-9500-65AAD177040D}" name="Description:" dataDxfId="2"/>
+    <tableColumn id="5" xr3:uid="{7DF12235-1193-B146-9500-65AAD177040D}" name="Description:" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium6" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -826,8 +826,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CEAB2FAD-92B8-DB4D-AB4C-9159AFD8911A}">
   <dimension ref="A1:G16"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D29" sqref="D29"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D17" sqref="D17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -837,18 +837,18 @@
   <sheetData>
     <row r="1" spans="1:7" ht="19" x14ac:dyDescent="0.25">
       <c r="A1" s="21" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B1" s="21"/>
       <c r="C1" s="21"/>
       <c r="D1" s="21"/>
       <c r="E1" s="21"/>
       <c r="F1" s="3" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="G1" s="19">
         <f ca="1">NOW()</f>
-        <v>43483.434360069441</v>
+        <v>43487.466467129627</v>
       </c>
     </row>
     <row r="3" spans="1:7" ht="36" customHeight="1" x14ac:dyDescent="0.2">
@@ -960,7 +960,7 @@
         <v>17</v>
       </c>
       <c r="B13" s="7" t="s">
-        <v>22</v>
+        <v>62</v>
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.2">
@@ -989,7 +989,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EFFE341A-F7C8-3F43-AC32-216069D199D4}">
   <dimension ref="A1:E11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A12" sqref="A12"/>
     </sheetView>
   </sheetViews>
@@ -1003,7 +1003,7 @@
   <sheetData>
     <row r="1" spans="1:5" ht="26" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.2">
@@ -1011,13 +1011,13 @@
         <v>5</v>
       </c>
       <c r="B3" s="8" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C3" s="8" t="s">
         <v>3</v>
       </c>
       <c r="D3" s="8" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="E3" s="8" t="s">
         <v>4</v>
@@ -1025,146 +1025,146 @@
     </row>
     <row r="4" spans="1:5" ht="50" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="11" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B4" s="12" t="s">
+        <v>25</v>
+      </c>
+      <c r="C4" s="10" t="s">
         <v>26</v>
-      </c>
-      <c r="C4" s="10" t="s">
-        <v>27</v>
       </c>
       <c r="D4" s="12" t="str">
         <f>"-1 and 1"</f>
         <v>-1 and 1</v>
       </c>
       <c r="E4" s="11" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="5" spans="1:5" ht="50" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="11" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B5" s="12" t="s">
+        <v>29</v>
+      </c>
+      <c r="C5" s="10" t="s">
         <v>30</v>
       </c>
-      <c r="C5" s="10" t="s">
+      <c r="D5" s="12" t="str">
+        <f t="shared" ref="D5:D11" si="0">"-32,768 .. 32,767"</f>
+        <v>-32,768 .. 32,767</v>
+      </c>
+      <c r="E5" s="11" t="s">
         <v>31</v>
-      </c>
-      <c r="D5" s="12" t="str">
-        <f>"-32,768 .. 32,767"</f>
-        <v>-32,768 .. 32,767</v>
-      </c>
-      <c r="E5" s="11" t="s">
-        <v>32</v>
       </c>
     </row>
     <row r="6" spans="1:5" ht="50" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="11" t="s">
+        <v>33</v>
+      </c>
+      <c r="B6" s="12" t="s">
         <v>34</v>
       </c>
-      <c r="B6" s="12" t="s">
+      <c r="C6" s="10" t="s">
+        <v>30</v>
+      </c>
+      <c r="D6" s="12" t="str">
+        <f t="shared" si="0"/>
+        <v>-32,768 .. 32,767</v>
+      </c>
+      <c r="E6" s="11" t="s">
         <v>35</v>
-      </c>
-      <c r="C6" s="10" t="s">
-        <v>31</v>
-      </c>
-      <c r="D6" s="12" t="str">
-        <f>"-32,768 .. 32,767"</f>
-        <v>-32,768 .. 32,767</v>
-      </c>
-      <c r="E6" s="11" t="s">
-        <v>36</v>
       </c>
     </row>
     <row r="7" spans="1:5" ht="68" x14ac:dyDescent="0.2">
       <c r="A7" s="11" t="s">
+        <v>36</v>
+      </c>
+      <c r="B7" s="12" t="s">
+        <v>34</v>
+      </c>
+      <c r="C7" s="10" t="s">
         <v>37</v>
       </c>
-      <c r="B7" s="12" t="s">
-        <v>35</v>
-      </c>
-      <c r="C7" s="10" t="s">
-        <v>38</v>
-      </c>
       <c r="D7" s="12" t="str">
-        <f>"-32,768 .. 32,767"</f>
+        <f t="shared" si="0"/>
         <v>-32,768 .. 32,767</v>
       </c>
       <c r="E7" s="11" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="8" spans="1:5" ht="50" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="11" t="s">
+        <v>38</v>
+      </c>
+      <c r="B8" s="12" t="s">
         <v>39</v>
       </c>
-      <c r="B8" s="12" t="s">
+      <c r="C8" s="10" t="s">
         <v>40</v>
       </c>
-      <c r="C8" s="10" t="s">
+      <c r="D8" s="12" t="str">
+        <f t="shared" si="0"/>
+        <v>-32,768 .. 32,767</v>
+      </c>
+      <c r="E8" s="11" t="s">
         <v>41</v>
-      </c>
-      <c r="D8" s="12" t="str">
-        <f>"-32,768 .. 32,767"</f>
-        <v>-32,768 .. 32,767</v>
-      </c>
-      <c r="E8" s="11" t="s">
-        <v>42</v>
       </c>
     </row>
     <row r="9" spans="1:5" ht="50" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="11" t="s">
+        <v>43</v>
+      </c>
+      <c r="B9" s="12" t="s">
         <v>44</v>
       </c>
-      <c r="B9" s="12" t="s">
+      <c r="C9" s="10" t="s">
         <v>45</v>
       </c>
-      <c r="C9" s="10" t="s">
+      <c r="D9" s="12" t="str">
+        <f t="shared" si="0"/>
+        <v>-32,768 .. 32,767</v>
+      </c>
+      <c r="E9" s="11" t="s">
         <v>46</v>
-      </c>
-      <c r="D9" s="12" t="str">
-        <f>"-32,768 .. 32,767"</f>
-        <v>-32,768 .. 32,767</v>
-      </c>
-      <c r="E9" s="11" t="s">
-        <v>47</v>
       </c>
     </row>
     <row r="10" spans="1:5" ht="50" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="11" t="s">
+        <v>56</v>
+      </c>
+      <c r="B10" s="12" t="s">
         <v>57</v>
       </c>
-      <c r="B10" s="12" t="s">
+      <c r="C10" s="10" t="s">
+        <v>30</v>
+      </c>
+      <c r="D10" s="12" t="str">
+        <f t="shared" si="0"/>
+        <v>-32,768 .. 32,767</v>
+      </c>
+      <c r="E10" s="11" t="s">
         <v>58</v>
-      </c>
-      <c r="C10" s="10" t="s">
-        <v>31</v>
-      </c>
-      <c r="D10" s="12" t="str">
-        <f>"-32,768 .. 32,767"</f>
-        <v>-32,768 .. 32,767</v>
-      </c>
-      <c r="E10" s="11" t="s">
-        <v>59</v>
       </c>
     </row>
     <row r="11" spans="1:5" ht="50" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="11" t="s">
+        <v>59</v>
+      </c>
+      <c r="B11" s="12" t="s">
         <v>60</v>
       </c>
-      <c r="B11" s="12" t="s">
+      <c r="C11" s="10" t="s">
+        <v>30</v>
+      </c>
+      <c r="D11" s="12" t="str">
+        <f t="shared" si="0"/>
+        <v>-32,768 .. 32,767</v>
+      </c>
+      <c r="E11" s="11" t="s">
         <v>61</v>
-      </c>
-      <c r="C11" s="10" t="s">
-        <v>31</v>
-      </c>
-      <c r="D11" s="12" t="str">
-        <f>"-32,768 .. 32,767"</f>
-        <v>-32,768 .. 32,767</v>
-      </c>
-      <c r="E11" s="11" t="s">
-        <v>62</v>
       </c>
     </row>
   </sheetData>
@@ -1193,7 +1193,7 @@
   <sheetData>
     <row r="1" spans="1:5" ht="26" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.2">
@@ -1201,13 +1201,13 @@
         <v>5</v>
       </c>
       <c r="B3" s="8" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C3" s="8" t="s">
         <v>3</v>
       </c>
       <c r="D3" s="8" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="E3" s="8" t="s">
         <v>4</v>
@@ -1215,10 +1215,10 @@
     </row>
     <row r="4" spans="1:5" ht="50" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="11" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B4" s="12" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C4" s="10">
         <v>-32.768000000000001</v>
@@ -1227,15 +1227,15 @@
         <v>-32.768000000000001</v>
       </c>
       <c r="E4" s="9" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="5" spans="1:5" ht="50" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="11" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B5" s="12" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C5" s="10">
         <v>0</v>
@@ -1244,15 +1244,15 @@
         <v>0</v>
       </c>
       <c r="E5" s="9" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="6" spans="1:5" ht="50" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="11" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B6" s="12" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C6" s="10">
         <v>0</v>
@@ -1261,7 +1261,7 @@
         <v>0</v>
       </c>
       <c r="E6" s="9" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added ICC tester and fixed typo in xlsx
</commit_message>
<xml_diff>
--- a/05_design/communication_protocol_MCU_NavU/com_protocol_MCU_NavU.xlsx
+++ b/05_design/communication_protocol_MCU_NavU/com_protocol_MCU_NavU.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10115"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10123"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Volumes/Macintosh SD/Github/ADAS/05_design/communication_protocol_MCU_NavU/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E49AE96C-7E30-0E48-AF84-FFFBFBB090A9}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{035079CF-E19E-2441-B348-B3666C25E094}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="9700" yWindow="460" windowWidth="22600" windowHeight="17440" xr2:uid="{17E85F93-DC07-064E-BD90-F4BCCAC86647}"/>
+    <workbookView xWindow="17680" yWindow="460" windowWidth="13620" windowHeight="17440" activeTab="1" xr2:uid="{17E85F93-DC07-064E-BD90-F4BCCAC86647}"/>
   </bookViews>
   <sheets>
     <sheet name="Structure" sheetId="1" r:id="rId1"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="63">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="64">
   <si>
     <t>To exchange data between the Navigation Unit (NavU) and the Motor Control Unit (MCU) a serial communication protocol is used.</t>
   </si>
@@ -222,6 +222,9 @@
   </si>
   <si>
     <t>The length of message is always 6 bytes including STX and TTX.</t>
+  </si>
+  <si>
+    <t>0x08</t>
   </si>
 </sst>
 </file>
@@ -826,7 +829,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CEAB2FAD-92B8-DB4D-AB4C-9159AFD8911A}">
   <dimension ref="A1:G16"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D17" sqref="D17"/>
     </sheetView>
   </sheetViews>
@@ -848,7 +851,7 @@
       </c>
       <c r="G1" s="19">
         <f ca="1">NOW()</f>
-        <v>43487.466467129627</v>
+        <v>43489.776421296294</v>
       </c>
     </row>
     <row r="3" spans="1:7" ht="36" customHeight="1" x14ac:dyDescent="0.2">
@@ -989,8 +992,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EFFE341A-F7C8-3F43-AC32-216069D199D4}">
   <dimension ref="A1:E11"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A12" sqref="A12"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1082,7 +1085,7 @@
         <v>36</v>
       </c>
       <c r="B7" s="12" t="s">
-        <v>34</v>
+        <v>39</v>
       </c>
       <c r="C7" s="10" t="s">
         <v>37</v>
@@ -1100,7 +1103,7 @@
         <v>38</v>
       </c>
       <c r="B8" s="12" t="s">
-        <v>39</v>
+        <v>44</v>
       </c>
       <c r="C8" s="10" t="s">
         <v>40</v>
@@ -1118,7 +1121,7 @@
         <v>43</v>
       </c>
       <c r="B9" s="12" t="s">
-        <v>44</v>
+        <v>57</v>
       </c>
       <c r="C9" s="10" t="s">
         <v>45</v>
@@ -1136,7 +1139,7 @@
         <v>56</v>
       </c>
       <c r="B10" s="12" t="s">
-        <v>57</v>
+        <v>60</v>
       </c>
       <c r="C10" s="10" t="s">
         <v>30</v>
@@ -1154,7 +1157,7 @@
         <v>59</v>
       </c>
       <c r="B11" s="12" t="s">
-        <v>60</v>
+        <v>63</v>
       </c>
       <c r="C11" s="10" t="s">
         <v>30</v>

</xml_diff>